<commit_message>
FIx bank loan example
</commit_message>
<xml_diff>
--- a/opt/Bank-loans.xlsx
+++ b/opt/Bank-loans.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boyko\proj\data\opt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E07F9C99-DDDA-446C-90BD-1FA88D4228DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{72B9AC16-B4E2-471F-B96B-F4D2ED5B4EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{F0FB0EF5-A071-4DCC-8119-A6F19BFB6251}"/>
   </bookViews>
   <sheets>
-    <sheet name="Answer Report 1" sheetId="21" r:id="rId1"/>
-    <sheet name="Sensitivity Report 1" sheetId="22" r:id="rId2"/>
-    <sheet name="Limits Report 1" sheetId="23" r:id="rId3"/>
+    <sheet name="Answer Report 1" sheetId="24" r:id="rId1"/>
+    <sheet name="Sensitivity Report 1" sheetId="25" r:id="rId2"/>
+    <sheet name="Limits Report 1" sheetId="26" r:id="rId3"/>
     <sheet name="Model" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
@@ -155,9 +155,6 @@
     <t>Engine: Simplex LP</t>
   </si>
   <si>
-    <t>Solution Time: 0.094 Seconds.</t>
-  </si>
-  <si>
     <t>Solver Options</t>
   </si>
   <si>
@@ -323,6 +320,9 @@
     <t>Upper</t>
   </si>
   <si>
+    <t>Solution Time: 0.078 Seconds.</t>
+  </si>
+  <si>
     <t>$C$15&lt;=$D$15</t>
   </si>
   <si>
@@ -356,13 +356,13 @@
     <t>Home Loans &gt;= 50% of Consumer, Automobile, and Home Loans</t>
   </si>
   <si>
-    <t>Worksheet: [Bank-leans.xlsx]Model</t>
-  </si>
-  <si>
-    <t>Report Created: 3/13/2025 11:52:19 PM</t>
-  </si>
-  <si>
-    <t>Report Created: 3/13/2025 11:52:20 PM</t>
+    <t>Worksheet: [Bank-loans.xlsx]Model</t>
+  </si>
+  <si>
+    <t>Report Created: 3/14/2025 12:11:28 AM</t>
+  </si>
+  <si>
+    <t>Report Created: 3/14/2025 12:11:29 AM</t>
   </si>
 </sst>
 </file>
@@ -840,10 +840,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{167B0F6F-F4B6-422C-9E80-037F3A639AB3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{925D313B-8F0C-45EE-A722-077173ED81AF}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -890,7 +890,7 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -901,36 +901,36 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="D15" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="E15" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -938,7 +938,7 @@
         <v>85</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D16" s="9">
         <v>0.9964799999999997</v>
@@ -949,50 +949,50 @@
     </row>
     <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="D20" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="E20" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="7" t="s">
-        <v>33</v>
-      </c>
       <c r="F20" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B21" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="D21" s="10">
+        <v>0</v>
+      </c>
+      <c r="E21" s="10">
+        <v>0</v>
+      </c>
+      <c r="F21" s="8" t="s">
         <v>42</v>
-      </c>
-      <c r="D21" s="10">
-        <v>0</v>
-      </c>
-      <c r="E21" s="10">
-        <v>0</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B22" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>45</v>
-      </c>
       <c r="D22" s="10">
         <v>0</v>
       </c>
@@ -1000,15 +1000,15 @@
         <v>0</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B23" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>47</v>
       </c>
       <c r="D23" s="10">
         <v>7.1999999999999984</v>
@@ -1017,16 +1017,16 @@
         <v>7.1999999999999984</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B24" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>49</v>
-      </c>
       <c r="D24" s="10">
         <v>0</v>
       </c>
@@ -1034,15 +1034,15 @@
         <v>0</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>51</v>
       </c>
       <c r="D25" s="9">
         <v>4.8</v>
@@ -1051,7 +1051,7 @@
         <v>4.8</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1061,30 +1061,30 @@
     </row>
     <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>31</v>
-      </c>
       <c r="D29" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="F29" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="G29" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B30" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D30" s="10">
         <v>11.999999999999998</v>
@@ -1093,7 +1093,7 @@
         <v>81</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G30" s="8">
         <v>0</v>
@@ -1101,10 +1101,10 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B31" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D31" s="13">
         <v>0.31199999999999994</v>
@@ -1113,7 +1113,7 @@
         <v>86</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G31" s="8">
         <v>0.16799999999999998</v>
@@ -1121,10 +1121,10 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B32" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D32" s="10">
         <v>4.8</v>
@@ -1133,7 +1133,7 @@
         <v>82</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G32" s="10">
         <v>0</v>
@@ -1144,7 +1144,7 @@
         <v>87</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D33" s="9">
         <v>7.1999999999999984</v>
@@ -1153,7 +1153,7 @@
         <v>88</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G33" s="9">
         <v>3.5999999999999992</v>
@@ -1165,7 +1165,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDA0CE59-5D2A-4639-825C-2441BE1C86F5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA917B4-3BA1-40DE-BA99-42FA43D9B440}">
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -1183,7 +1183,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -1198,69 +1198,69 @@
     </row>
     <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>31</v>
-      </c>
       <c r="D8" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G8" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>42</v>
-      </c>
       <c r="D9" s="8">
         <v>0</v>
       </c>
       <c r="E9" s="8">
-        <v>-6.0399999999999954E-2</v>
+        <v>-5.1399999999999973E-2</v>
       </c>
       <c r="F9" s="8">
-        <v>2.6000000000000023E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="G9" s="8">
-        <v>6.0399999999999954E-2</v>
+        <v>5.1399999999999973E-2</v>
       </c>
       <c r="H9" s="8">
         <v>1E+30</v>
@@ -1268,22 +1268,22 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>45</v>
-      </c>
       <c r="D10" s="8">
         <v>0</v>
       </c>
       <c r="E10" s="8">
-        <v>-3.5500000000000004E-2</v>
+        <v>-3.5499999999999976E-2</v>
       </c>
       <c r="F10" s="8">
-        <v>5.0899999999999973E-2</v>
+        <v>5.0900000000000001E-2</v>
       </c>
       <c r="G10" s="8">
-        <v>3.5500000000000004E-2</v>
+        <v>3.5499999999999976E-2</v>
       </c>
       <c r="H10" s="8">
         <v>1E+30</v>
@@ -1291,10 +1291,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>47</v>
       </c>
       <c r="D11" s="8">
         <v>7.1999999999999984</v>
@@ -1314,10 +1314,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>49</v>
       </c>
       <c r="D12" s="8">
         <v>0</v>
@@ -1337,10 +1337,10 @@
     </row>
     <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>51</v>
       </c>
       <c r="D13" s="6">
         <v>4.8</v>
@@ -1367,50 +1367,50 @@
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
       <c r="D16" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="12" t="s">
-        <v>31</v>
-      </c>
       <c r="D17" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G17" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H17" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="H17" s="12" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D18" s="8">
         <v>11.999999999999998</v>
@@ -1430,10 +1430,10 @@
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D19" s="8">
         <v>0.31199999999999994</v>
@@ -1453,10 +1453,10 @@
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D20" s="8">
         <v>4.8</v>
@@ -1479,7 +1479,7 @@
         <v>87</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D21" s="6">
         <v>7.1999999999999984</v>
@@ -1503,7 +1503,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F87706A3-A3A8-44A8-9F0A-F88C62F30599}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C03D130-ED0B-47BE-BC7E-AD2D50E0753C}">
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -1524,7 +1524,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -1541,19 +1541,19 @@
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="11"/>
       <c r="C6" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D6" s="11"/>
     </row>
     <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>31</v>
-      </c>
       <c r="D7" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1561,7 +1561,7 @@
         <v>85</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" s="9">
         <v>0.9964799999999997</v>
@@ -1571,51 +1571,51 @@
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="11"/>
       <c r="C11" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D11" s="11"/>
       <c r="F11" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>31</v>
-      </c>
       <c r="D12" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F12" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="G12" s="12" t="s">
-        <v>79</v>
-      </c>
       <c r="I12" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="J12" s="12" t="s">
         <v>78</v>
-      </c>
-      <c r="J12" s="12" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>42</v>
       </c>
       <c r="D13" s="10">
         <v>0</v>
@@ -1635,10 +1635,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>44</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>45</v>
       </c>
       <c r="D14" s="10">
         <v>0</v>
@@ -1658,10 +1658,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>47</v>
       </c>
       <c r="D15" s="10">
         <v>7.1999999999999984</v>
@@ -1681,10 +1681,10 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>49</v>
       </c>
       <c r="D16" s="10">
         <v>0</v>
@@ -1704,10 +1704,10 @@
     </row>
     <row r="17" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>51</v>
       </c>
       <c r="D17" s="9">
         <v>4.8</v>
@@ -1735,7 +1735,7 @@
   <dimension ref="B1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1793,7 +1793,7 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>0.14000000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="D3">
         <v>0.13</v>

</xml_diff>